<commit_message>
Bestellliste aktualisiert + MotorControl.c
</commit_message>
<xml_diff>
--- a/documents/Bestellung_Micromouse_2022_01.xlsx
+++ b/documents/Bestellung_Micromouse_2022_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\LRZ_Sync_Share\Joshua\Studium\TUM\Semester-3-WS2122\Micromouse\Micromouse\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mibet\Documents\Uni\micromouse\Micromouse\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{36C583CC-1248-4165-B562-A2817CB920C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A5940DE-7341-4BAA-96B5-FB2AF41B30F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11893" tabRatio="989"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS-online" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Lieferant: RS</t>
   </si>
@@ -202,13 +202,22 @@
   <si>
     <t>Voltage
 Regulator</t>
+  </si>
+  <si>
+    <t>700 Ohm</t>
+  </si>
+  <si>
+    <t>LED low current, red, surface mount</t>
+  </si>
+  <si>
+    <t>749-SM0805HCL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -229,6 +238,12 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -259,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -305,9 +320,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -676,40 +692,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.8203125" customWidth="1"/>
-    <col min="3" max="3" width="35.05859375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1171875" customWidth="1"/>
-    <col min="6" max="6" width="17.64453125" customWidth="1"/>
-    <col min="7" max="7" width="6.76171875" customWidth="1"/>
-    <col min="8" max="8" width="19.5859375" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.7" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" ht="25.35" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" s="12" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
@@ -735,7 +751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="25.35" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>48</v>
       </c>
@@ -760,7 +776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="38" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>46</v>
       </c>
@@ -785,7 +801,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="38" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>45</v>
       </c>
@@ -812,7 +828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="50.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>47</v>
       </c>
@@ -839,7 +855,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>49</v>
       </c>
@@ -849,7 +865,7 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>50</v>
       </c>
@@ -859,17 +875,26 @@
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>51</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>52</v>
       </c>
@@ -880,14 +905,14 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="25.35" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="5"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="E16" s="2" t="s">
         <v>21</v>
@@ -898,84 +923,84 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="F17">
         <f t="shared" ref="F17:F29" si="1">D17*E17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="F18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="F19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="F20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="F21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F29">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -993,40 +1018,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.8203125" customWidth="1"/>
-    <col min="2" max="2" width="35.05859375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1171875" customWidth="1"/>
-    <col min="5" max="5" width="17.64453125" customWidth="1"/>
-    <col min="6" max="6" width="6.76171875" customWidth="1"/>
-    <col min="7" max="7" width="19.5859375" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.7" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="13" customFormat="1" ht="25.35" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>37</v>
       </c>
@@ -1049,7 +1074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" s="17" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>38</v>
       </c>
@@ -1073,49 +1098,64 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0.49</v>
+      </c>
       <c r="E8">
         <f t="shared" ref="E8:E9" si="0">D8*C8</f>
-        <v>0</v>
+        <v>0.98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10">
-        <f t="shared" ref="E8:E14" si="1">D10*C10</f>
+        <f t="shared" ref="E10:E14" si="1">D10*C10</f>
         <v>0</v>
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
       <c r="E14">
         <f t="shared" si="1"/>
@@ -1123,89 +1163,89 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="2">
         <f>SUM(E7:E13)</f>
-        <v>20.170000000000002</v>
+        <v>21.150000000000002</v>
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16">
         <f t="shared" ref="E16:E28" si="2">C16*D16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:5" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="5:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1223,34 +1263,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.8203125" customWidth="1"/>
-    <col min="4" max="4" width="35.05859375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1171875" customWidth="1"/>
-    <col min="7" max="7" width="17.64453125" customWidth="1"/>
-    <col min="8" max="8" width="6.76171875" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1268,7 +1308,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="3:8" ht="42.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:8" ht="42.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1287,7 +1327,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="3:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1345,7 @@
         <v>14.38</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="76.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:8" ht="76.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -1323,7 +1363,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="10" spans="3:8" ht="31.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:8" ht="31.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -1337,7 +1377,7 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="11" spans="3:8" ht="42.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:8" ht="42.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>15</v>
       </c>
@@ -1355,7 +1395,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="12" spans="3:8" ht="31.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:8" ht="31.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>17</v>
       </c>
@@ -1373,7 +1413,7 @@
         <v>6.7700000000000005</v>
       </c>
     </row>
-    <row r="13" spans="3:8" ht="42.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:8" ht="42.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>19</v>
       </c>
@@ -1391,14 +1431,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="3:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="5"/>
       <c r="G14">
         <f>E14*F14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1407,79 +1447,79 @@
         <v>46.18</v>
       </c>
     </row>
-    <row r="16" spans="3:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G16">
         <f t="shared" ref="G16:G28" si="0">E16*F16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:7" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="7:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G28">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
code structure + bestellliste updated
</commit_message>
<xml_diff>
--- a/documents/Bestellung_Micromouse_2022_01.xlsx
+++ b/documents/Bestellung_Micromouse_2022_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mibet\Documents\Uni\micromouse\Micromouse\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C8C75-62D3-4002-A6C8-A80C67BF0832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D98EC2-660E-4283-8723-B4149A1A4976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12132" yWindow="1644" windowWidth="12960" windowHeight="8964" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS-online" sheetId="2" r:id="rId1"/>
@@ -209,9 +209,6 @@
     <t>SOD123</t>
   </si>
   <si>
-    <t xml:space="preserve">LED 3MM </t>
-  </si>
-  <si>
     <t xml:space="preserve">Push-Button </t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>449-LFXTAL036034REEL</t>
   </si>
   <si>
-    <t>593-LTH3MM12VFR4500</t>
-  </si>
-  <si>
     <t>682-1131</t>
   </si>
   <si>
@@ -309,6 +303,12 @@
   </si>
   <si>
     <t>1 kOhm, 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED 5MM </t>
+  </si>
+  <si>
+    <t>593-LTH5MM12VFR4400</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -968,7 +968,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>56</v>
@@ -990,7 +990,7 @@
         <v>50</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>55</v>
@@ -1012,7 +1012,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -1034,10 +1034,10 @@
         <v>50</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="15" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1286,20 +1286,20 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.96299999999999997</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.96299999999999997</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="F9" t="s">
         <v>30</v>
@@ -1308,10 +1308,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1330,10 +1330,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1349,10 +1349,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1387,10 +1387,10 @@
     </row>
     <row r="14" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="15" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>9</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="16" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1444,10 +1444,10 @@
     </row>
     <row r="17" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1463,10 +1463,10 @@
     </row>
     <row r="18" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E19" s="2">
         <f>SUM(E7:E13)</f>
-        <v>32.21</v>
+        <v>32.218000000000004</v>
       </c>
       <c r="G19" s="6"/>
     </row>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="21" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="22" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1522,10 +1522,10 @@
     </row>
     <row r="23" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>1</v>

</xml_diff>